<commit_message>
Added new factors and adjusted values, including dependencies between factors
</commit_message>
<xml_diff>
--- a/germany_strikedata.xlsx
+++ b/germany_strikedata.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexi\OneDrive\DS FHNW\FS25\wer\OMC\simulation_of_the_delivery_time\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://fhnw365-my.sharepoint.com/personal/mykhailo_andrusiak_students_fhnw_ch/Documents/FHNW/WER/simulation_of_the_delivery_time/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E920921-FE47-4E07-A11E-8BD7E105E9BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="64" documentId="13_ncr:1_{3E920921-FE47-4E07-A11E-8BD7E105E9BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{24FDEC9A-ADE2-C54B-884F-69A5A76DA981}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-1155" windowWidth="29040" windowHeight="15720" xr2:uid="{D19E7103-73BE-4B4C-956A-9FE499A31348}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{D19E7103-73BE-4B4C-956A-9FE499A31348}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$7:$H$7</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="68">
   <si>
     <t xml:space="preserve">logistik strikes in germany 2014 -2024 </t>
   </si>
@@ -280,20 +283,16 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">(51.1 - 28 - 1) /10 = </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>2.21</t>
-    </r>
+    <t>Till 3 days delays</t>
+  </si>
+  <si>
+    <t>(51.1 - 28 - 1) /12 = 1.84</t>
+  </si>
+  <si>
+    <t>More than 3 days delays</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
@@ -301,13 +300,6 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -329,6 +321,13 @@
       <color theme="10"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -369,17 +368,16 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -388,25 +386,33 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="15" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -742,504 +748,604 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC7F067A-8AF6-49E2-9E1D-A19C41AAB437}">
-  <dimension ref="A3:H28"/>
+  <dimension ref="A3:H45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="G42" sqref="G42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="13.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" style="5"/>
-    <col min="2" max="2" width="18.85546875" customWidth="1"/>
-    <col min="3" max="3" width="13.85546875" style="6"/>
-    <col min="5" max="6" width="13.85546875" style="6"/>
-    <col min="7" max="7" width="100.7109375" customWidth="1"/>
-    <col min="8" max="8" width="41.7109375" customWidth="1"/>
+    <col min="1" max="1" width="13.83203125" style="4"/>
+    <col min="2" max="2" width="18.83203125" customWidth="1"/>
+    <col min="3" max="3" width="13.83203125" style="5"/>
+    <col min="5" max="6" width="13.83203125" style="5"/>
+    <col min="7" max="7" width="100.6640625" customWidth="1"/>
+    <col min="8" max="8" width="41.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="4"/>
+    <row r="3" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="3"/>
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="4"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-    </row>
-    <row r="5" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="17"/>
-      <c r="B5" s="18" t="s">
+      <c r="C3" s="3"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+    </row>
+    <row r="5" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="15"/>
+      <c r="B5" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="17" t="s">
+      <c r="C5" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="18" t="s">
+      <c r="D5" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="E5" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="17" t="s">
+      <c r="F5" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="G5" s="18" t="s">
+      <c r="G5" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="H5" s="18" t="s">
+      <c r="H5" s="16" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="4"/>
-      <c r="B6" s="2" t="s">
+    <row r="6" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="3"/>
+      <c r="C6" s="6"/>
+      <c r="E6" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="3"/>
+      <c r="B7" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C6" s="7"/>
-      <c r="E6" s="7" t="s">
+      <c r="C7" s="6"/>
+      <c r="E7" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F6" s="7" t="s">
+      <c r="F7" s="6" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
-      <c r="C7" s="7"/>
-      <c r="E7" s="7" t="s">
+    <row r="8" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="14">
+        <v>7</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="F8" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="G8" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="14">
         <v>3</v>
       </c>
-      <c r="F7" s="7" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="16">
+      <c r="B9" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="9">
         <v>1</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="F9" s="9">
+        <v>1</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="H9" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="14">
+        <v>9</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="9">
+        <v>1</v>
+      </c>
+      <c r="F10" s="9">
+        <v>1</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="H10" s="11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="14">
+        <v>11</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="9">
+        <v>1</v>
+      </c>
+      <c r="F11" s="9">
+        <v>1</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="H11" s="11" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="4">
+        <v>12</v>
+      </c>
+      <c r="B12" t="s">
+        <v>43</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" s="5">
+        <v>1</v>
+      </c>
+      <c r="F12" s="5">
+        <v>1</v>
+      </c>
+      <c r="G12" t="s">
+        <v>47</v>
+      </c>
+      <c r="H12" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="14">
+        <v>13</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13" s="9">
+        <v>1</v>
+      </c>
+      <c r="F13" s="9">
+        <v>1</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="H13" s="11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="4">
+        <v>14</v>
+      </c>
+      <c r="B14" t="s">
+        <v>50</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" s="5">
+        <v>1</v>
+      </c>
+      <c r="F14" s="5">
+        <v>1</v>
+      </c>
+      <c r="G14" t="s">
+        <v>51</v>
+      </c>
+      <c r="H14" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" s="14">
+        <v>1</v>
+      </c>
+      <c r="B15" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="10">
+      <c r="C15" s="9">
         <v>9</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="D15" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="10">
+      <c r="E15" s="9">
         <v>17</v>
       </c>
-      <c r="F8" s="10">
+      <c r="F15" s="9">
         <v>1.9</v>
       </c>
-      <c r="G8" s="9" t="s">
+      <c r="G15" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="H8" s="11" t="s">
+      <c r="H15" s="10" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="5">
+    <row r="16" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="4">
+        <v>8</v>
+      </c>
+      <c r="B16" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16" t="s">
+        <v>31</v>
+      </c>
+      <c r="E16" s="5">
         <v>2</v>
       </c>
-      <c r="B9" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D9" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" s="6">
-        <v>3</v>
-      </c>
-      <c r="F9" s="6">
-        <v>3</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="16">
-        <v>3</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="E10" s="10">
-        <v>1</v>
-      </c>
-      <c r="F10" s="10">
-        <v>1</v>
-      </c>
-      <c r="G10" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="H10" s="9" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="5">
-        <v>4</v>
-      </c>
-      <c r="B11" t="s">
-        <v>27</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D11" t="s">
-        <v>8</v>
-      </c>
-      <c r="E11" s="6">
-        <v>4</v>
-      </c>
-      <c r="F11" s="6">
-        <v>4</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H11" s="8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="16">
-        <v>5</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="D12" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="E12" s="10">
-        <v>28</v>
-      </c>
-      <c r="F12" s="10">
-        <v>28</v>
-      </c>
-      <c r="G12" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="H12" s="13" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="5">
-        <v>6</v>
-      </c>
-      <c r="B13" t="s">
-        <v>29</v>
-      </c>
-      <c r="C13" s="6">
-        <v>3</v>
-      </c>
-      <c r="D13" t="s">
-        <v>15</v>
-      </c>
-      <c r="E13" s="6">
-        <v>11</v>
-      </c>
-      <c r="F13" s="6">
-        <v>3.7</v>
-      </c>
-      <c r="G13" t="s">
-        <v>24</v>
-      </c>
-      <c r="H13" s="8" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="16">
-        <v>7</v>
-      </c>
-      <c r="B14" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="C14" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="D14" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="E14" s="10">
-        <v>0.5</v>
-      </c>
-      <c r="F14" s="10">
-        <v>0.5</v>
-      </c>
-      <c r="G14" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="H14" s="9" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="5">
-        <v>8</v>
-      </c>
-      <c r="B15" t="s">
-        <v>34</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D15" t="s">
-        <v>31</v>
-      </c>
-      <c r="E15" s="6">
+      <c r="F16" s="5">
         <v>2</v>
       </c>
-      <c r="F15" s="6">
-        <v>2</v>
-      </c>
-      <c r="G15" t="s">
+      <c r="G16" t="s">
         <v>35</v>
       </c>
-      <c r="H15" s="8" t="s">
+      <c r="H16" s="7" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="16">
-        <v>9</v>
-      </c>
-      <c r="B16" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="C16" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="D16" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="E16" s="10">
-        <v>1</v>
-      </c>
-      <c r="F16" s="10">
-        <v>1</v>
-      </c>
-      <c r="G16" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="H16" s="13" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="5">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" s="4">
         <v>10</v>
       </c>
       <c r="B17" t="s">
         <v>39</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="C17" s="5" t="s">
         <v>18</v>
       </c>
       <c r="D17" t="s">
         <v>21</v>
       </c>
-      <c r="E17" s="6">
+      <c r="E17" s="5">
         <v>2</v>
       </c>
-      <c r="F17" s="6">
+      <c r="F17" s="5">
         <v>2</v>
       </c>
       <c r="G17" t="s">
         <v>40</v>
       </c>
-      <c r="H17" s="8" t="s">
+      <c r="H17" s="7" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="18" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="16">
+    <row r="18" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="4">
+        <v>2</v>
+      </c>
+      <c r="B18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D18" t="s">
+        <v>8</v>
+      </c>
+      <c r="E18" s="5">
+        <v>3</v>
+      </c>
+      <c r="F18" s="5">
+        <v>3</v>
+      </c>
+      <c r="G18" t="s">
+        <v>10</v>
+      </c>
+      <c r="H18" t="s">
         <v>11</v>
       </c>
-      <c r="B18" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="C18" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="D18" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="E18" s="10">
-        <v>1</v>
-      </c>
-      <c r="F18" s="10">
-        <v>1</v>
-      </c>
-      <c r="G18" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="H18" s="13" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="5">
-        <v>12</v>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" s="4">
+        <v>6</v>
       </c>
       <c r="B19" t="s">
-        <v>43</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>18</v>
+        <v>29</v>
+      </c>
+      <c r="C19" s="5">
+        <v>3</v>
       </c>
       <c r="D19" t="s">
         <v>15</v>
       </c>
-      <c r="E19" s="6">
-        <v>1</v>
-      </c>
-      <c r="F19" s="6">
-        <v>1</v>
+      <c r="E19" s="5">
+        <v>11</v>
+      </c>
+      <c r="F19" s="5">
+        <v>3.7</v>
       </c>
       <c r="G19" t="s">
-        <v>47</v>
-      </c>
-      <c r="H19" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="H19" s="7" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="16">
-        <v>13</v>
-      </c>
-      <c r="B20" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="C20" s="10" t="s">
+    <row r="20" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="4">
+        <v>4</v>
+      </c>
+      <c r="B20" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D20" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="E20" s="10">
-        <v>1</v>
-      </c>
-      <c r="F20" s="10">
-        <v>1</v>
-      </c>
-      <c r="G20" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="H20" s="13" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="5">
-        <v>14</v>
-      </c>
-      <c r="B21" t="s">
-        <v>50</v>
-      </c>
-      <c r="C21" s="6" t="s">
+      <c r="D20" t="s">
+        <v>8</v>
+      </c>
+      <c r="E20" s="5">
+        <v>4</v>
+      </c>
+      <c r="F20" s="5">
+        <v>4</v>
+      </c>
+      <c r="G20" t="s">
+        <v>20</v>
+      </c>
+      <c r="H20" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" s="14">
+        <v>5</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C21" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="D21" t="s">
-        <v>8</v>
-      </c>
-      <c r="E21" s="6">
-        <v>1</v>
-      </c>
-      <c r="F21" s="6">
-        <v>1</v>
-      </c>
-      <c r="G21" t="s">
-        <v>51</v>
-      </c>
-      <c r="H21" s="8" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F22" s="5"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E24" s="6" t="s">
+      <c r="D21" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E21" s="9">
+        <v>28</v>
+      </c>
+      <c r="F21" s="9">
+        <v>28</v>
+      </c>
+      <c r="G21" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H21" s="11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F22" s="4"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E23" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="F23" s="18"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E24" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="F24" s="5">
+      <c r="F24" s="4">
         <f>SUM(F8:F23)</f>
         <v>51.1</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E25" s="6" t="s">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E25" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="F25" s="5">
+      <c r="F25" s="4">
         <v>3.65</v>
       </c>
       <c r="G25" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E26" s="6" t="s">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E26" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="F26" s="5">
-        <v>2.21</v>
+      <c r="F26" s="17">
+        <f>(F24-28-1)/12</f>
+        <v>1.8416666666666668</v>
       </c>
       <c r="G26" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E27" s="5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E27" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="F27" s="5">
+      <c r="F27" s="4">
         <v>6.5700000000000003E-3</v>
       </c>
       <c r="G27" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="G28" t="s">
         <v>60</v>
       </c>
     </row>
+    <row r="34" spans="5:6" x14ac:dyDescent="0.2">
+      <c r="E34" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="F34" s="18"/>
+    </row>
+    <row r="35" spans="5:6" x14ac:dyDescent="0.2">
+      <c r="E35" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F35" s="19">
+        <f>SUM(F8:F18)</f>
+        <v>15.4</v>
+      </c>
+    </row>
+    <row r="36" spans="5:6" x14ac:dyDescent="0.2">
+      <c r="E36" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="F36" s="19">
+        <f>AVERAGE(F8:F18)</f>
+        <v>1.4000000000000001</v>
+      </c>
+    </row>
+    <row r="37" spans="5:6" x14ac:dyDescent="0.2">
+      <c r="E37" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="F37" s="19">
+        <f>(F35-0.5-3)/9</f>
+        <v>1.3222222222222222</v>
+      </c>
+    </row>
+    <row r="38" spans="5:6" x14ac:dyDescent="0.2">
+      <c r="E38" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="F38" s="19">
+        <f>(11+8)/(365*10)</f>
+        <v>5.2054794520547945E-3</v>
+      </c>
+    </row>
+    <row r="41" spans="5:6" x14ac:dyDescent="0.2">
+      <c r="E41" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="F41" s="18"/>
+    </row>
+    <row r="42" spans="5:6" x14ac:dyDescent="0.2">
+      <c r="E42" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F42" s="19">
+        <f>SUM(F19:F21)</f>
+        <v>35.700000000000003</v>
+      </c>
+    </row>
+    <row r="43" spans="5:6" x14ac:dyDescent="0.2">
+      <c r="E43" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="F43" s="19">
+        <f>AVERAGE(F19:F21)</f>
+        <v>11.9</v>
+      </c>
+    </row>
+    <row r="44" spans="5:6" x14ac:dyDescent="0.2">
+      <c r="E44" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="F44" s="19">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="45" spans="5:6" x14ac:dyDescent="0.2">
+      <c r="E45" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="F45" s="19">
+        <f>(3+2)/(365*10)</f>
+        <v>1.3698630136986301E-3</v>
+      </c>
+    </row>
   </sheetData>
+  <autoFilter ref="A7:H7" xr:uid="{AC7F067A-8AF6-49E2-9E1D-A19C41AAB437}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A8:H21">
+      <sortCondition ref="F7:F21"/>
+    </sortState>
+  </autoFilter>
+  <mergeCells count="3">
+    <mergeCell ref="E41:F41"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E23:F23"/>
+  </mergeCells>
   <hyperlinks>
-    <hyperlink ref="H8" r:id="rId1" location="Tarifstreit_und_Streiks_2014/2015" xr:uid="{B53E2F89-6395-44B1-9E65-F1ED34C962A1}"/>
-    <hyperlink ref="H11" r:id="rId2" xr:uid="{F8097F3D-1958-4CA3-B87A-CCFB92FBDD05}"/>
-    <hyperlink ref="H12" r:id="rId3" xr:uid="{63F65B85-20D0-45F5-A491-65FF00E05445}"/>
-    <hyperlink ref="H13" r:id="rId4" xr:uid="{12A4E0E6-5E28-42AB-A726-B78B4C537B52}"/>
-    <hyperlink ref="H15" r:id="rId5" xr:uid="{38D2BDBA-D759-470D-A159-9651F03BB6C4}"/>
-    <hyperlink ref="H16" r:id="rId6" xr:uid="{1D747FA6-4944-45F2-BFEE-A75A27CF21DD}"/>
+    <hyperlink ref="H15" r:id="rId1" location="Tarifstreit_und_Streiks_2014/2015" xr:uid="{B53E2F89-6395-44B1-9E65-F1ED34C962A1}"/>
+    <hyperlink ref="H20" r:id="rId2" xr:uid="{F8097F3D-1958-4CA3-B87A-CCFB92FBDD05}"/>
+    <hyperlink ref="H21" r:id="rId3" xr:uid="{63F65B85-20D0-45F5-A491-65FF00E05445}"/>
+    <hyperlink ref="H19" r:id="rId4" xr:uid="{12A4E0E6-5E28-42AB-A726-B78B4C537B52}"/>
+    <hyperlink ref="H16" r:id="rId5" xr:uid="{38D2BDBA-D759-470D-A159-9651F03BB6C4}"/>
+    <hyperlink ref="H10" r:id="rId6" xr:uid="{1D747FA6-4944-45F2-BFEE-A75A27CF21DD}"/>
     <hyperlink ref="H17" r:id="rId7" xr:uid="{0165AAA9-9E60-4052-A9FA-6EA3A9163E75}"/>
-    <hyperlink ref="H19" r:id="rId8" xr:uid="{CB4DFC47-9A51-4744-A89F-55BF729BE327}"/>
-    <hyperlink ref="H20" r:id="rId9" xr:uid="{BE03828C-57B9-44DF-A1C8-E0E82155F763}"/>
-    <hyperlink ref="H21" r:id="rId10" xr:uid="{0BAC5F06-2099-4AF4-88AB-7267E0F748D4}"/>
+    <hyperlink ref="H12" r:id="rId8" xr:uid="{CB4DFC47-9A51-4744-A89F-55BF729BE327}"/>
+    <hyperlink ref="H13" r:id="rId9" xr:uid="{BE03828C-57B9-44DF-A1C8-E0E82155F763}"/>
+    <hyperlink ref="H14" r:id="rId10" xr:uid="{0BAC5F06-2099-4AF4-88AB-7267E0F748D4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId11"/>

</xml_diff>

<commit_message>
corrected statisitcs in strikedata and edited the strikedata in simulation_delivery.ipynb
</commit_message>
<xml_diff>
--- a/germany_strikedata.xlsx
+++ b/germany_strikedata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://fhnw365-my.sharepoint.com/personal/mykhailo_andrusiak_students_fhnw_ch/Documents/FHNW/WER/simulation_of_the_delivery_time/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f6d213be512b1d25/DS FHNW/FS25/wer/OMC/simulation_of_the_delivery_time/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="64" documentId="13_ncr:1_{3E920921-FE47-4E07-A11E-8BD7E105E9BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{24FDEC9A-ADE2-C54B-884F-69A5A76DA981}"/>
+  <xr:revisionPtr revIDLastSave="243" documentId="13_ncr:1_{3E920921-FE47-4E07-A11E-8BD7E105E9BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8CF07CD3-8A8B-4E3C-8641-5981F9AABEB0}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{D19E7103-73BE-4B4C-956A-9FE499A31348}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{D19E7103-73BE-4B4C-956A-9FE499A31348}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="80">
   <si>
     <t xml:space="preserve">logistik strikes in germany 2014 -2024 </t>
   </si>
@@ -48,9 +48,6 @@
   </si>
   <si>
     <t>remarks</t>
-  </si>
-  <si>
-    <t>! day= 8 h</t>
   </si>
   <si>
     <t>day = 24h</t>
@@ -243,9 +240,6 @@
   </si>
   <si>
     <t>substrike</t>
-  </si>
-  <si>
-    <t>3650 * 0.00657 = 23.9805</t>
   </si>
   <si>
     <r>
@@ -264,12 +258,18 @@
     </r>
   </si>
   <si>
-    <t>gestutzes mean</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">51.1/14 = </t>
-    </r>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Gestutzes Mittel oder Werte von 0.5 bis 3 verwenden?</t>
+  </si>
+  <si>
+    <t>Gestutzes Mittel</t>
+  </si>
+  <si>
+    <t>19 Occurances (11 + 8)</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <b/>
@@ -279,20 +279,181 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>3.65</t>
-    </r>
-  </si>
-  <si>
-    <t>Till 3 days delays</t>
-  </si>
-  <si>
-    <t>(51.1 - 28 - 1) /12 = 1.84</t>
-  </si>
-  <si>
-    <t>More than 3 days delays</t>
-  </si>
-  <si>
-    <t>Total</t>
+      <t xml:space="preserve">24 Occurances </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">(14 + (9-1) +( 3-1)) </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">51.1/ 24 = </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2.1291</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">(51.1 - 28 - 0.5) / 22   = </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1.02727</t>
+    </r>
+  </si>
+  <si>
+    <t>Artihemtisches Mittel oder Modalwert hier besser geeignet?</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Short Strike: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Until 3 days delays</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Long Strike:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> More than 3 days delays</t>
+    </r>
+  </si>
+  <si>
+    <t>P( short strike)</t>
+  </si>
+  <si>
+    <t>P(long strike)</t>
+  </si>
+  <si>
+    <t>5 Occurances (3 + 2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> day !=  8 h</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">30.5 / 19 = </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1.6052</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">19 / (365*10) = </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0.0052</t>
+    </r>
+  </si>
+  <si>
+    <t>Wieviele Kommastellen?</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">43 / 5 = </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>8.6</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>5 / (365*10)  =</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 0.0014</t>
+    </r>
+  </si>
+  <si>
+    <t>x</t>
   </si>
 </sst>
 </file>
@@ -331,7 +492,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -356,8 +517,38 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -365,12 +556,92 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -404,15 +675,72 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -748,23 +1076,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC7F067A-8AF6-49E2-9E1D-A19C41AAB437}">
-  <dimension ref="A3:H45"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A3:I41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="G42" sqref="G42"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L26" sqref="L26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="13.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="13.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.83203125" style="4"/>
-    <col min="2" max="2" width="18.83203125" customWidth="1"/>
-    <col min="3" max="3" width="13.83203125" style="5"/>
-    <col min="5" max="6" width="13.83203125" style="5"/>
-    <col min="7" max="7" width="100.6640625" customWidth="1"/>
-    <col min="8" max="8" width="41.6640625" customWidth="1"/>
+    <col min="1" max="1" width="13.85546875" style="4"/>
+    <col min="2" max="2" width="18.85546875" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" style="5"/>
+    <col min="4" max="4" width="16.140625" customWidth="1"/>
+    <col min="5" max="5" width="19" style="5" customWidth="1"/>
+    <col min="6" max="6" width="17.140625" style="5" customWidth="1"/>
+    <col min="7" max="7" width="100.7109375" customWidth="1"/>
+    <col min="8" max="8" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" s="1" t="s">
         <v>0</v>
@@ -773,566 +1106,647 @@
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
     </row>
-    <row r="5" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="15"/>
       <c r="B5" s="16" t="s">
         <v>1</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F5" s="15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G5" s="16" t="s">
         <v>2</v>
       </c>
       <c r="H5" s="16" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="C6" s="6"/>
-      <c r="E6" s="6" t="s">
-        <v>3</v>
+      <c r="E6" s="20" t="s">
+        <v>73</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C7" s="6"/>
-      <c r="E7" s="6" t="s">
-        <v>4</v>
+      <c r="E7" s="20" t="s">
+        <v>3</v>
       </c>
       <c r="F7" s="6" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="8" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="14">
         <v>7</v>
       </c>
       <c r="B8" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="C8" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="E8" s="9">
+      <c r="E8" s="18">
         <v>0.5</v>
       </c>
       <c r="F8" s="9">
         <v>0.5</v>
       </c>
       <c r="G8" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="H8" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="H8" s="8" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I8" s="8" t="str">
+        <f>""</f>
+        <v/>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="14">
         <v>3</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" s="9">
+        <v>7</v>
+      </c>
+      <c r="E9" s="18">
         <v>1</v>
       </c>
       <c r="F9" s="9">
         <v>1</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H9" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+      <c r="I9" t="str">
+        <f>""</f>
+        <v/>
+      </c>
+    </row>
+    <row r="10" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="14">
         <v>9</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="E10" s="9">
+        <v>7</v>
+      </c>
+      <c r="E10" s="18">
         <v>1</v>
       </c>
       <c r="F10" s="9">
         <v>1</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H10" s="11" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+        <v>22</v>
+      </c>
+      <c r="I10" t="str">
+        <f>""</f>
+        <v/>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="14">
         <v>11</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="E11" s="9">
+        <v>14</v>
+      </c>
+      <c r="E11" s="18">
         <v>1</v>
       </c>
       <c r="F11" s="9">
         <v>1</v>
       </c>
       <c r="G11" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="H11" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="H11" s="11" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I11" t="str">
+        <f>""</f>
+        <v/>
+      </c>
+    </row>
+    <row r="12" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D12" t="s">
-        <v>15</v>
-      </c>
-      <c r="E12" s="5">
+        <v>14</v>
+      </c>
+      <c r="E12" s="18">
         <v>1</v>
       </c>
-      <c r="F12" s="5">
+      <c r="F12" s="21">
         <v>1</v>
       </c>
       <c r="G12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+      <c r="I12" t="str">
+        <f>""</f>
+        <v/>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="14">
         <v>13</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="E13" s="9">
+        <v>14</v>
+      </c>
+      <c r="E13" s="18">
         <v>1</v>
       </c>
       <c r="F13" s="9">
         <v>1</v>
       </c>
       <c r="G13" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H13" s="11" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+      <c r="I13" t="str">
+        <f>""</f>
+        <v/>
+      </c>
+    </row>
+    <row r="14" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>14</v>
       </c>
       <c r="B14" t="s">
+        <v>49</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" s="18">
+        <v>1</v>
+      </c>
+      <c r="F14" s="21">
+        <v>1</v>
+      </c>
+      <c r="G14" t="s">
         <v>50</v>
       </c>
-      <c r="C14" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D14" t="s">
-        <v>8</v>
-      </c>
-      <c r="E14" s="5">
-        <v>1</v>
-      </c>
-      <c r="F14" s="5">
-        <v>1</v>
-      </c>
-      <c r="G14" t="s">
+      <c r="H14" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="H14" s="7" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I14" t="str">
+        <f>""</f>
+        <v/>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="14">
         <v>1</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C15" s="9">
         <v>9</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="E15" s="9">
+        <v>14</v>
+      </c>
+      <c r="E15" s="18">
         <v>17</v>
       </c>
       <c r="F15" s="9">
         <v>1.9</v>
       </c>
       <c r="G15" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H15" s="10" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+      <c r="I15" t="str">
+        <f>""</f>
+        <v/>
+      </c>
+    </row>
+    <row r="16" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>8</v>
       </c>
       <c r="B16" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D16" t="s">
+        <v>30</v>
+      </c>
+      <c r="E16" s="18">
+        <v>2</v>
+      </c>
+      <c r="F16" s="21">
+        <v>2</v>
+      </c>
+      <c r="G16" t="s">
         <v>34</v>
       </c>
-      <c r="C16" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D16" t="s">
-        <v>31</v>
-      </c>
-      <c r="E16" s="5">
-        <v>2</v>
-      </c>
-      <c r="F16" s="5">
-        <v>2</v>
-      </c>
-      <c r="G16" t="s">
+      <c r="H16" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="H16" s="7" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I16" t="str">
+        <f>""</f>
+        <v/>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>10</v>
       </c>
       <c r="B17" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D17" t="s">
+        <v>20</v>
+      </c>
+      <c r="E17" s="18">
+        <v>2</v>
+      </c>
+      <c r="F17" s="21">
+        <v>2</v>
+      </c>
+      <c r="G17" t="s">
         <v>39</v>
       </c>
-      <c r="C17" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D17" t="s">
-        <v>21</v>
-      </c>
-      <c r="E17" s="5">
-        <v>2</v>
-      </c>
-      <c r="F17" s="5">
-        <v>2</v>
-      </c>
-      <c r="G17" t="s">
+      <c r="H17" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="H17" s="7" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I17" t="str">
+        <f>""</f>
+        <v/>
+      </c>
+    </row>
+    <row r="18" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <v>2</v>
       </c>
       <c r="B18" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D18" t="s">
         <v>7</v>
       </c>
-      <c r="C18" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D18" t="s">
-        <v>8</v>
-      </c>
-      <c r="E18" s="5">
+      <c r="E18" s="18">
         <v>3</v>
       </c>
-      <c r="F18" s="5">
+      <c r="F18" s="21">
         <v>3</v>
       </c>
       <c r="G18" t="s">
+        <v>9</v>
+      </c>
+      <c r="H18" t="s">
         <v>10</v>
       </c>
-      <c r="H18" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I18" t="str">
+        <f>""</f>
+        <v/>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
         <v>6</v>
       </c>
       <c r="B19" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C19" s="5">
         <v>3</v>
       </c>
       <c r="D19" t="s">
-        <v>15</v>
-      </c>
-      <c r="E19" s="5">
+        <v>14</v>
+      </c>
+      <c r="E19" s="19">
         <v>11</v>
       </c>
-      <c r="F19" s="5">
+      <c r="F19" s="21">
         <v>3.7</v>
       </c>
       <c r="G19" t="s">
+        <v>23</v>
+      </c>
+      <c r="H19" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="H19" s="7" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I19" t="str">
+        <f>""</f>
+        <v/>
+      </c>
+    </row>
+    <row r="20" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <v>4</v>
       </c>
       <c r="B20" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C20" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D20" t="s">
+        <v>7</v>
+      </c>
+      <c r="E20" s="19">
+        <v>4</v>
+      </c>
+      <c r="F20" s="21">
+        <v>4</v>
+      </c>
+      <c r="G20" t="s">
+        <v>19</v>
+      </c>
+      <c r="H20" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D20" t="s">
-        <v>8</v>
-      </c>
-      <c r="E20" s="5">
-        <v>4</v>
-      </c>
-      <c r="F20" s="5">
-        <v>4</v>
-      </c>
-      <c r="G20" t="s">
-        <v>20</v>
-      </c>
-      <c r="H20" s="7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I20" t="str">
+        <f>""</f>
+        <v/>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="14">
         <v>5</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="E21" s="9">
+        <v>20</v>
+      </c>
+      <c r="E21" s="19">
         <v>28</v>
       </c>
       <c r="F21" s="9">
         <v>28</v>
       </c>
       <c r="G21" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="H21" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="H21" s="11" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I21" t="str">
+        <f>""</f>
+        <v/>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F22" s="4"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="E23" s="18" t="s">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E23" s="36" t="s">
+        <v>60</v>
+      </c>
+      <c r="F23" s="41"/>
+      <c r="G23" s="35"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E24" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="F24" s="37">
+        <f>SUM(E8:E23)</f>
+        <v>73.5</v>
+      </c>
+      <c r="G24" s="27" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E25" s="28" t="s">
+        <v>53</v>
+      </c>
+      <c r="F25" s="38">
+        <v>2.13</v>
+      </c>
+      <c r="G25" s="27" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E26" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="F26" s="39">
+        <f>(F24-28-0.5)/22</f>
+        <v>2.0454545454545454</v>
+      </c>
+      <c r="G26" s="27" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E27" s="30" t="s">
+        <v>54</v>
+      </c>
+      <c r="F27" s="40">
+        <v>6.6E-3</v>
+      </c>
+      <c r="G27" s="32" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G28" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="F23" s="18"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="E24" s="5" t="s">
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G29" s="42" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E30" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="F30" s="23"/>
+      <c r="G30" s="24" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E31" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="F31" s="26">
+        <f>SUM(E8:E18)</f>
+        <v>30.5</v>
+      </c>
+      <c r="G31" s="27" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E32" s="28" t="s">
         <v>53</v>
       </c>
-      <c r="F24" s="4">
-        <f>SUM(F8:F23)</f>
-        <v>51.1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="E25" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="F25" s="4">
-        <v>3.65</v>
-      </c>
-      <c r="G25" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="E26" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="F26" s="17">
-        <f>(F24-28-1)/12</f>
-        <v>1.8416666666666668</v>
-      </c>
-      <c r="G26" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="E27" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="F27" s="4">
-        <v>6.5700000000000003E-3</v>
-      </c>
-      <c r="G27" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="G28" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="34" spans="5:6" x14ac:dyDescent="0.2">
-      <c r="E34" s="18" t="s">
-        <v>64</v>
-      </c>
-      <c r="F34" s="18"/>
-    </row>
-    <row r="35" spans="5:6" x14ac:dyDescent="0.2">
-      <c r="E35" s="5" t="s">
+      <c r="F32" s="29">
+        <v>1.61</v>
+      </c>
+      <c r="G32" s="27" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="33" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E33" s="25"/>
+      <c r="F33" s="26"/>
+      <c r="G33" s="27"/>
+    </row>
+    <row r="34" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E34" s="30" t="s">
+        <v>70</v>
+      </c>
+      <c r="F34" s="31">
+        <v>5.1999999999999998E-3</v>
+      </c>
+      <c r="G34" s="32" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="35" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="H35" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="37" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E37" s="33" t="s">
+        <v>69</v>
+      </c>
+      <c r="F37" s="34"/>
+      <c r="G37" s="35"/>
+    </row>
+    <row r="38" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E38" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="F38" s="26">
+        <f>SUM(E19:E21)</f>
+        <v>43</v>
+      </c>
+      <c r="G38" s="27" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="39" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E39" s="28" t="s">
         <v>53</v>
       </c>
-      <c r="F35" s="19">
-        <f>SUM(F8:F18)</f>
-        <v>15.4</v>
-      </c>
-    </row>
-    <row r="36" spans="5:6" x14ac:dyDescent="0.2">
-      <c r="E36" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="F36" s="19">
-        <f>AVERAGE(F8:F18)</f>
-        <v>1.4000000000000001</v>
-      </c>
-    </row>
-    <row r="37" spans="5:6" x14ac:dyDescent="0.2">
-      <c r="E37" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="F37" s="19">
-        <f>(F35-0.5-3)/9</f>
-        <v>1.3222222222222222</v>
-      </c>
-    </row>
-    <row r="38" spans="5:6" x14ac:dyDescent="0.2">
-      <c r="E38" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="F38" s="19">
-        <f>(11+8)/(365*10)</f>
-        <v>5.2054794520547945E-3</v>
-      </c>
-    </row>
-    <row r="41" spans="5:6" x14ac:dyDescent="0.2">
-      <c r="E41" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="F41" s="18"/>
-    </row>
-    <row r="42" spans="5:6" x14ac:dyDescent="0.2">
-      <c r="E42" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="F42" s="19">
-        <f>SUM(F19:F21)</f>
-        <v>35.700000000000003</v>
-      </c>
-    </row>
-    <row r="43" spans="5:6" x14ac:dyDescent="0.2">
-      <c r="E43" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="F43" s="19">
-        <f>AVERAGE(F19:F21)</f>
-        <v>11.9</v>
-      </c>
-    </row>
-    <row r="44" spans="5:6" x14ac:dyDescent="0.2">
-      <c r="E44" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="F44" s="19">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="45" spans="5:6" x14ac:dyDescent="0.2">
-      <c r="E45" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="F45" s="19">
-        <f>(3+2)/(365*10)</f>
-        <v>1.3698630136986301E-3</v>
+      <c r="F39" s="29">
+        <v>8.6</v>
+      </c>
+      <c r="G39" s="27" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="40" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E40" s="25"/>
+      <c r="F40" s="26"/>
+      <c r="G40" s="27"/>
+    </row>
+    <row r="41" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E41" s="30" t="s">
+        <v>71</v>
+      </c>
+      <c r="F41" s="31">
+        <v>1.4E-3</v>
+      </c>
+      <c r="G41" s="32" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A7:H7" xr:uid="{AC7F067A-8AF6-49E2-9E1D-A19C41AAB437}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A8:H21">
-      <sortCondition ref="F7:F21"/>
+      <sortCondition ref="F7"/>
     </sortState>
   </autoFilter>
   <mergeCells count="3">
-    <mergeCell ref="E41:F41"/>
-    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E30:F30"/>
     <mergeCell ref="E23:F23"/>
   </mergeCells>
   <hyperlinks>
@@ -1347,7 +1761,7 @@
     <hyperlink ref="H13" r:id="rId9" xr:uid="{BE03828C-57B9-44DF-A1C8-E0E82155F763}"/>
     <hyperlink ref="H14" r:id="rId10" xr:uid="{0BAC5F06-2099-4AF4-88AB-7267E0F748D4}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId11"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="58" orientation="landscape" r:id="rId11"/>
 </worksheet>
 </file>
</xml_diff>